<commit_message>
Update CFG costs spreadsheet
</commit_message>
<xml_diff>
--- a/CfgCreateProcess/CFG process create costs.xlsx
+++ b/CfgCreateProcess/CFG process create costs.xlsx
@@ -16,18 +16,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Function count</t>
   </si>
   <si>
     <t>ms</t>
+  </si>
+  <si>
+    <t>34D</t>
+  </si>
+  <si>
+    <t>13BCD</t>
+  </si>
+  <si>
+    <t>2744D</t>
+  </si>
+  <si>
+    <t>3ACCD</t>
+  </si>
+  <si>
+    <t>4E54D</t>
+  </si>
+  <si>
+    <t>61DCD</t>
+  </si>
+  <si>
+    <t>7564D</t>
+  </si>
+  <si>
+    <t>88ECD</t>
+  </si>
+  <si>
+    <t>9C74D</t>
+  </si>
+  <si>
+    <t>AFFCD</t>
+  </si>
+  <si>
+    <t>C384D</t>
+  </si>
+  <si>
+    <t>D70CD</t>
+  </si>
+  <si>
+    <t>EA94D</t>
+  </si>
+  <si>
+    <t>FE1CD</t>
+  </si>
+  <si>
+    <t>111A4D</t>
+  </si>
+  <si>
+    <t>1252CD</t>
+  </si>
+  <si>
+    <t>138B4D</t>
+  </si>
+  <si>
+    <t>Guard CF function count</t>
+  </si>
+  <si>
+    <t>CFG count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -57,8 +117,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -91,14 +158,14 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -107,76 +174,71 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$18</c:f>
+              <c:f>Sheet1!$C$2:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>845</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>80845</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200</c:v>
+                  <c:v>160845</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300</c:v>
+                  <c:v>240845</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>400</c:v>
+                  <c:v>320845</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500</c:v>
+                  <c:v>400845</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>600</c:v>
+                  <c:v>480845</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>700</c:v>
+                  <c:v>560845</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>800</c:v>
+                  <c:v>640845</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>900</c:v>
+                  <c:v>720845</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1000</c:v>
+                  <c:v>800845</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1100</c:v>
+                  <c:v>880845</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1200</c:v>
+                  <c:v>960845</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1300</c:v>
+                  <c:v>1040845</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1400</c:v>
+                  <c:v>1120845</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1500</c:v>
+                  <c:v>1200845</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1600</c:v>
+                  <c:v>1280845</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$18</c:f>
+              <c:f>Sheet1!$D$2:$D$18</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>3.7669999999999999</c:v>
@@ -232,7 +294,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -242,14 +304,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="219412352"/>
-        <c:axId val="219410816"/>
+        <c:axId val="277414656"/>
+        <c:axId val="275639296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="219412352"/>
+        <c:axId val="277414656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1600"/>
+          <c:max val="1300000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -264,7 +327,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Functions per class</a:t>
+                  <a:t>Guard CF function count</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -276,12 +339,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="219410816"/>
+        <c:crossAx val="275639296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="400000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="219410816"/>
+        <c:axId val="275639296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -299,7 +363,211 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Create Process (ms)</a:t>
+                  <a:t>CreateProcess time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="277414656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$24:$C$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>845</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80845</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160845</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240845</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>320845</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>480845</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>560845</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>640845</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>720845</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>800845</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>880845</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>960845</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1040845</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1120845</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1200845</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1280845</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$24:$E$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1.9408760908414529</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4552858058343019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8544854598845832</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3400239807808703</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.990359411775394</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.537429593538059</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.070905388309647</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.463829505278692</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.144857530851326</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.678576815340907</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26.392764159898068</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.975852015083181</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>31.481677210720523</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>34.425194262342224</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37.442409110525993</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40.311884103822287</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43.050249708915743</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="146637568"/>
+        <c:axId val="146635776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="146637568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1200000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Guard CF function count</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -311,7 +579,43 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="219412352"/>
+        <c:crossAx val="146635776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="400000"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="146635776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>sqrt(CreateProcess time (ms))</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146637568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -332,20 +636,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>90488</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -355,6 +659,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>433386</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -650,157 +984,716 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f>HEX2DEC(B2)</f>
+        <v>845</v>
+      </c>
+      <c r="D2" s="2">
         <v>3.7669999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>100</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C18" si="0">HEX2DEC(B3)</f>
+        <v>80845</v>
+      </c>
+      <c r="D3" s="2">
         <v>11.939</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>200</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>160845</v>
+      </c>
+      <c r="D4" s="2">
         <v>34.274999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>300</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>240845</v>
+      </c>
+      <c r="D5" s="2">
         <v>69.555999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>400</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>320845</v>
+      </c>
+      <c r="D6" s="2">
         <v>120.788</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>500</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>400845</v>
+      </c>
+      <c r="D7" s="2">
         <v>183.262</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>600</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>480845</v>
+      </c>
+      <c r="D8" s="2">
         <v>258.274</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>700</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>560845</v>
+      </c>
+      <c r="D9" s="2">
         <v>340.91300000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>800</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>640845</v>
+      </c>
+      <c r="D10" s="2">
         <v>447.10500000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>900</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>720845</v>
+      </c>
+      <c r="D11" s="2">
         <v>560.67499999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1000</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>800845</v>
+      </c>
+      <c r="D12" s="2">
         <v>696.57799999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1100</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>880845</v>
+      </c>
+      <c r="D13" s="2">
         <v>839.6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1200</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>960845</v>
+      </c>
+      <c r="D14" s="2">
         <v>991.096</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1300</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1040845</v>
+      </c>
+      <c r="D15" s="2">
         <v>1185.0940000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1400</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>1120845</v>
+      </c>
+      <c r="D16" s="2">
         <v>1401.934</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1500</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>1200845</v>
+      </c>
+      <c r="D17" s="2">
         <v>1625.048</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1600</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>1280845</v>
+      </c>
+      <c r="D18" s="2">
         <v>1853.3240000000001</v>
       </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <f>HEX2DEC(B24)</f>
+        <v>845</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3.7669999999999999</v>
+      </c>
+      <c r="E24">
+        <f>SQRT(D24)</f>
+        <v>1.9408760908414529</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>100</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:C40" si="1">HEX2DEC(B25)</f>
+        <v>80845</v>
+      </c>
+      <c r="D25" s="2">
+        <v>11.939</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ref="E25:E40" si="2">SQRT(D25)</f>
+        <v>3.4552858058343019</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>200</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>160845</v>
+      </c>
+      <c r="D26" s="2">
+        <v>34.274999999999999</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>5.8544854598845832</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>300</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>240845</v>
+      </c>
+      <c r="D27" s="2">
+        <v>69.555999999999997</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>8.3400239807808703</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>400</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>320845</v>
+      </c>
+      <c r="D28" s="2">
+        <v>120.788</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>10.990359411775394</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>500</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>400845</v>
+      </c>
+      <c r="D29" s="2">
+        <v>183.262</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>13.537429593538059</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>600</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>480845</v>
+      </c>
+      <c r="D30" s="2">
+        <v>258.274</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>16.070905388309647</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>700</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>560845</v>
+      </c>
+      <c r="D31" s="2">
+        <v>340.91300000000001</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>18.463829505278692</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>800</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>640845</v>
+      </c>
+      <c r="D32" s="2">
+        <v>447.10500000000002</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>21.144857530851326</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>900</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>720845</v>
+      </c>
+      <c r="D33" s="2">
+        <v>560.67499999999995</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>23.678576815340907</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1000</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>800845</v>
+      </c>
+      <c r="D34" s="2">
+        <v>696.57799999999997</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>26.392764159898068</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1100</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>880845</v>
+      </c>
+      <c r="D35" s="2">
+        <v>839.6</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>28.975852015083181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1200</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>960845</v>
+      </c>
+      <c r="D36" s="2">
+        <v>991.096</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>31.481677210720523</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1300</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>1040845</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1185.0940000000001</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>34.425194262342224</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1400</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>1120845</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1401.934</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>37.442409110525993</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1500</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>1200845</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1625.048</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>40.311884103822287</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1600</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>1280845</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1853.3240000000001</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>43.050249708915743</v>
+      </c>
+    </row>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>